<commit_message>
Before added .astypefloat for all logs in function
</commit_message>
<xml_diff>
--- a/Examples/Opx_Liq_Thermobarometry/Opx_Liq_Example.xlsx
+++ b/Examples/Opx_Liq_Thermobarometry/Opx_Liq_Example.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oregonstateuniversity-my.sharepoint.com/personal/wieserp_oregonstate_edu/Documents/Postdoc/PyMME/MyBarometers/Thermobar_outer/Examples/Opx_Liq_Thermobarometry/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Examples\Opx_Liq_Thermobarometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{F26DD648-3E2F-4F36-9F69-A527688E317C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1307B0E5-3CCA-45FB-B788-5FB7E601F2C1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900AF182-7A1F-4726-A2B6-37719B77B5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E8E7985B-3CF2-4EFE-9D4B-8895F7D277F0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="2" xr2:uid="{E8E7985B-3CF2-4EFE-9D4B-8895F7D277F0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Paired_Opx_Liq" sheetId="1" r:id="rId1"/>
+    <sheet name="Separate_Opxs" sheetId="2" r:id="rId2"/>
+    <sheet name="Separate_Liqs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -118,6 +120,42 @@
   </si>
   <si>
     <t>Pair5</t>
+  </si>
+  <si>
+    <t>Sample_ID_Opx</t>
+  </si>
+  <si>
+    <t>Opx1</t>
+  </si>
+  <si>
+    <t>Opx2</t>
+  </si>
+  <si>
+    <t>Opx3</t>
+  </si>
+  <si>
+    <t>Opx4</t>
+  </si>
+  <si>
+    <t>Opx5</t>
+  </si>
+  <si>
+    <t>Liquid1</t>
+  </si>
+  <si>
+    <t>Liquid2</t>
+  </si>
+  <si>
+    <t>Liquid3</t>
+  </si>
+  <si>
+    <t>Liquid4</t>
+  </si>
+  <si>
+    <t>Liquid5</t>
+  </si>
+  <si>
+    <t>Liquid6</t>
   </si>
 </sst>
 </file>
@@ -127,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +190,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -186,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -208,6 +258,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E477760D-8872-44D0-99F1-C56BCECBE94C}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="A1:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,4 +1017,547 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{936051E7-570A-41E5-80BB-63A8F3B850B8}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.77734375" customWidth="1"/>
+    <col min="11" max="11" width="19.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>55</v>
+      </c>
+      <c r="C2">
+        <v>0.34</v>
+      </c>
+      <c r="D2">
+        <v>1.5</v>
+      </c>
+      <c r="E2">
+        <v>11.3</v>
+      </c>
+      <c r="F2">
+        <v>0.24</v>
+      </c>
+      <c r="G2">
+        <v>30.7</v>
+      </c>
+      <c r="H2">
+        <v>0.9</v>
+      </c>
+      <c r="I2">
+        <v>0.01</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>52.7</v>
+      </c>
+      <c r="C3">
+        <v>0.15</v>
+      </c>
+      <c r="D3">
+        <v>8.1</v>
+      </c>
+      <c r="E3">
+        <v>8.48</v>
+      </c>
+      <c r="F3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G3">
+        <v>29.4</v>
+      </c>
+      <c r="H3">
+        <v>2.14</v>
+      </c>
+      <c r="I3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>53.2</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+      <c r="D4">
+        <v>7.4</v>
+      </c>
+      <c r="E4">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F4">
+        <v>0.13</v>
+      </c>
+      <c r="G4">
+        <v>29.2</v>
+      </c>
+      <c r="H4">
+        <v>2.37</v>
+      </c>
+      <c r="I4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>55.15</v>
+      </c>
+      <c r="C5">
+        <v>0.17</v>
+      </c>
+      <c r="D5">
+        <v>1.19</v>
+      </c>
+      <c r="E5">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.22</v>
+      </c>
+      <c r="G5">
+        <v>29.99</v>
+      </c>
+      <c r="H5">
+        <v>1.66</v>
+      </c>
+      <c r="I5">
+        <v>0.03</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>56.32</v>
+      </c>
+      <c r="C6">
+        <v>0.13</v>
+      </c>
+      <c r="D6">
+        <v>1.41</v>
+      </c>
+      <c r="E6">
+        <v>10.17</v>
+      </c>
+      <c r="F6">
+        <v>0.26</v>
+      </c>
+      <c r="G6">
+        <v>30.88</v>
+      </c>
+      <c r="H6">
+        <v>1.05</v>
+      </c>
+      <c r="I6">
+        <v>0.02</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F10AE9AE-D4E4-4C6F-8B69-1C198E860578}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6">
+        <v>51.1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.93</v>
+      </c>
+      <c r="D2" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="E2" s="6">
+        <v>8.91</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="G2" s="7">
+        <v>6.09</v>
+      </c>
+      <c r="H2" s="6">
+        <v>11.5</v>
+      </c>
+      <c r="I2" s="6">
+        <v>3.53</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="M2" s="6">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="6">
+        <v>51.5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1.19</v>
+      </c>
+      <c r="D3" s="6">
+        <v>19.2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.19</v>
+      </c>
+      <c r="G3" s="7">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="H3" s="6">
+        <v>10</v>
+      </c>
+      <c r="I3" s="6">
+        <v>3.72</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M3" s="6">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="6">
+        <v>59.1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.54</v>
+      </c>
+      <c r="D4" s="6">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5.22</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.19</v>
+      </c>
+      <c r="G4" s="7">
+        <v>3.25</v>
+      </c>
+      <c r="H4" s="6">
+        <v>7.45</v>
+      </c>
+      <c r="I4" s="6">
+        <v>4</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="M4" s="6">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="6">
+        <v>52.5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.98</v>
+      </c>
+      <c r="D5" s="6">
+        <v>19.2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>4.99</v>
+      </c>
+      <c r="H5" s="6">
+        <v>9.64</v>
+      </c>
+      <c r="I5" s="6">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M5" s="6">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="6">
+        <v>56.2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.34</v>
+      </c>
+      <c r="D6" s="6">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5.88</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2.58</v>
+      </c>
+      <c r="H6" s="6">
+        <v>7.18</v>
+      </c>
+      <c r="I6" s="6">
+        <v>6.02</v>
+      </c>
+      <c r="J6" s="6">
+        <v>1.02</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="M6" s="6">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6">
+        <v>51.3</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.93</v>
+      </c>
+      <c r="D7" s="6">
+        <v>17.2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>8.91</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="G7" s="7">
+        <v>6.09</v>
+      </c>
+      <c r="H7" s="6">
+        <v>11.5</v>
+      </c>
+      <c r="I7" s="6">
+        <v>4</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="M7" s="6">
+        <v>3.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>